<commit_message>
Added more error handling for empty/string/duplicate values, cleaned up functions
</commit_message>
<xml_diff>
--- a/orders_santa.xlsx
+++ b/orders_santa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyra\PycharmProjects\Assignment2_A01080450_A01170735\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE7A35F-FC5A-4BA4-BD82-55315810FFD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115582C8-6BF7-420E-AA91-5D103D252594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="1500" windowWidth="13545" windowHeight="11985" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
+    <workbookView xWindow="28935" yWindow="195" windowWidth="17040" windowHeight="14700" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>name</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Santas Workshop - Essentials Edition</t>
-  </si>
-  <si>
-    <t>Santas Workshop - Deluxe Edition</t>
   </si>
   <si>
     <t>C1230T</t>
@@ -495,9 +492,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC969572-FB28-418E-B89D-F0DD002AE5AA}">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -551,7 +548,7 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -575,25 +572,25 @@
         <v>15</v>
       </c>
       <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
         <v>26</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>27</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>28</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>29</v>
-      </c>
-      <c r="V1" t="s">
-        <v>30</v>
       </c>
       <c r="W1" t="s">
         <v>8</v>
       </c>
       <c r="X1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
@@ -603,9 +600,6 @@
       <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
@@ -613,19 +607,19 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K2">
         <v>10</v>
@@ -635,35 +629,29 @@
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
       <c r="E3">
         <v>5</v>
       </c>
       <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
         <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Finished commenting, did some cleanup
</commit_message>
<xml_diff>
--- a/orders_santa.xlsx
+++ b/orders_santa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyra\PycharmProjects\Assignment2_A01080450_A01170735\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115582C8-6BF7-420E-AA91-5D103D252594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31511CE5-4F48-40DA-A80D-676421F6CCB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28935" yWindow="195" windowWidth="17040" windowHeight="14700" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
+    <workbookView xWindow="29415" yWindow="1620" windowWidth="16980" windowHeight="13080" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>"string"</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,6 +603,9 @@
       <c r="B2" t="s">
         <v>17</v>
       </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
@@ -629,8 +635,14 @@
       <c r="A3">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
       <c r="C3" t="s">
         <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
       </c>
       <c r="E3">
         <v>5</v>

</xml_diff>